<commit_message>
Unification bulk RNA name (#1189)
* Updated enum 'bulk RNA' assay type to be 'bulk-RNA' across tools

* Updated for CI

* Updated Changelog to clean visualization
</commit_message>
<xml_diff>
--- a/docs/bulkrnaseq/bulkrnaseq-metadata.xlsx
+++ b/docs/bulkrnaseq/bulkrnaseq-metadata.xlsx
@@ -544,7 +544,7 @@
     <t>assay_type</t>
   </si>
   <si>
-    <t>bulk RNA</t>
+    <t>bulk-RNA</t>
   </si>
   <si>
     <t>analyte_class</t>
@@ -1110,7 +1110,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: sequence." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: bulk RNA." sqref="L2:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: bulk-RNA." sqref="L2:L1048576">
       <formula1>'assay_type list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: RNA." sqref="M2:M1048576">

</xml_diff>